<commit_message>
Version Final 03 fecha: 25/05/2023
</commit_message>
<xml_diff>
--- a/Script/Dataframes/df_Acuse_Presentacion.xlsx
+++ b/Script/Dataframes/df_Acuse_Presentacion.xlsx
@@ -446,17 +446,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Fecha_y_hora_presentacion</t>
+          <t>Fecha y hora presentacion</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Num_de_Operacion</t>
+          <t>Num de Operacion</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Periodo_de_declaracion</t>
+          <t>Periodo de declaracion</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -466,17 +466,17 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>total_a_pagar</t>
+          <t>total a pagar</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Vigente_hasta</t>
+          <t>Vigente hasta</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Linea_de_Captura</t>
+          <t>Linea de Captura</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Impuesto_a_favor</t>
+          <t>Impuesto a favor</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">

</xml_diff>